<commit_message>
Added_Abbott et al. 2021_details
</commit_message>
<xml_diff>
--- a/Lit_Review_Fig/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
+++ b/Lit_Review_Fig/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-modeling/Lit_Review_Fig/FireMeta_Rproj/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A775F8A7-556D-0A40-8CF8-BC34B9FA2EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DF4E397-DDE7-BF4E-9E6B-7B59BB406D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34660" yWindow="1960" windowWidth="30240" windowHeight="17360" activeTab="2" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
+    <workbookView xWindow="38920" yWindow="2200" windowWidth="30240" windowHeight="17360" activeTab="3" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
   </bookViews>
   <sheets>
     <sheet name="Study_info" sheetId="2" r:id="rId1"/>
     <sheet name="Study_info_filtered" sheetId="7" r:id="rId2"/>
-    <sheet name="Study_info_filtered_take_one" sheetId="8" r:id="rId3"/>
-    <sheet name="Exclusion" sheetId="3" r:id="rId4"/>
-    <sheet name="Original_meta_analysis" sheetId="4" r:id="rId5"/>
+    <sheet name="Study_info_filtered_V1" sheetId="8" r:id="rId3"/>
+    <sheet name="Study_info_filtered_V2" sheetId="9" r:id="rId4"/>
+    <sheet name="Exclusion" sheetId="3" r:id="rId5"/>
+    <sheet name="Original_meta_analysis" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5254" uniqueCount="1380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5743" uniqueCount="1383">
   <si>
     <t>Study</t>
   </si>
@@ -4258,6 +4259,15 @@
   </si>
   <si>
     <t>3 monthly concentrations</t>
+  </si>
+  <si>
+    <t>Four mile canyon - Colorado</t>
+  </si>
+  <si>
+    <t>Nantahala National Forest-NC</t>
+  </si>
+  <si>
+    <t>In_git_studies_folder</t>
   </si>
 </sst>
 </file>
@@ -4520,7 +4530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4610,6 +4620,7 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4929,7 +4940,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14096,7 +14107,7 @@
   <dimension ref="A1:AQ321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD49"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23455,8 +23466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90229B5-CF41-C440-BFCC-1DBDEC7AB338}">
   <dimension ref="A1:AQ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26079,6 +26090,2100 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AC9E00-AE6F-C745-827A-7F2C45C3ED66}">
+  <dimension ref="A1:AA42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18:P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="73"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" s="73" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="73"/>
+      <c r="B2" s="15" t="s">
+        <v>727</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1998</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>724</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="18"/>
+      <c r="N2" s="17" t="s">
+        <v>725</v>
+      </c>
+      <c r="O2" s="19">
+        <v>48.762999999999998</v>
+      </c>
+      <c r="P2" s="19">
+        <v>-114.226</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>5</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>726</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="73"/>
+      <c r="B3" s="15" t="s">
+        <v>681</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1992</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>692</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>733</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>734</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>731</v>
+      </c>
+      <c r="O3" s="22">
+        <v>49.667000000000002</v>
+      </c>
+      <c r="P3" s="22">
+        <v>-93.733000000000004</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>15</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>732</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="73"/>
+      <c r="B4" s="15" t="s">
+        <v>740</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2008</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>741</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>742</v>
+      </c>
+      <c r="O4" s="15">
+        <v>49.616667</v>
+      </c>
+      <c r="P4" s="15">
+        <v>-114.666667</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>3</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="73"/>
+      <c r="B5" s="27" t="s">
+        <v>750</v>
+      </c>
+      <c r="C5" s="27">
+        <v>2008</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>786</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>751</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>752</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="21" t="s">
+        <v>753</v>
+      </c>
+      <c r="O5" s="22">
+        <v>48.789253000000002</v>
+      </c>
+      <c r="P5" s="22">
+        <v>-113.79626500000001</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>4</v>
+      </c>
+      <c r="R5" s="23" t="s">
+        <v>754</v>
+      </c>
+      <c r="S5" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" s="27" t="s">
+        <v>755</v>
+      </c>
+      <c r="V5" s="27"/>
+    </row>
+    <row r="6" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="73"/>
+      <c r="B6" s="15" t="s">
+        <v>781</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2009</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>693</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>785</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>784</v>
+      </c>
+      <c r="O6" s="15">
+        <v>65.150000000000006</v>
+      </c>
+      <c r="P6" s="15">
+        <v>-147.5</v>
+      </c>
+      <c r="Q6" s="15">
+        <v>3</v>
+      </c>
+      <c r="S6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="73"/>
+      <c r="B7" s="15" t="s">
+        <v>790</v>
+      </c>
+      <c r="C7" s="15">
+        <v>2014</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>771</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>772</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="27"/>
+      <c r="N7" s="36" t="s">
+        <v>768</v>
+      </c>
+      <c r="O7" s="15">
+        <v>40.702464999999997</v>
+      </c>
+      <c r="P7" s="15">
+        <v>-105.241646</v>
+      </c>
+      <c r="Q7" s="15">
+        <v>1</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>791</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="73"/>
+      <c r="B8" s="27" t="s">
+        <v>827</v>
+      </c>
+      <c r="C8" s="27">
+        <v>2016</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>693</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>828</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>829</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="40" t="s">
+        <v>834</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>830</v>
+      </c>
+      <c r="O8" s="22">
+        <v>40.353888888</v>
+      </c>
+      <c r="P8" s="22">
+        <v>-105.583611111</v>
+      </c>
+      <c r="Q8" s="23">
+        <v>2</v>
+      </c>
+      <c r="R8" s="23" t="s">
+        <v>831</v>
+      </c>
+      <c r="S8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" s="27" t="s">
+        <v>832</v>
+      </c>
+      <c r="V8" s="27"/>
+    </row>
+    <row r="9" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="73"/>
+      <c r="B9" s="15" t="s">
+        <v>849</v>
+      </c>
+      <c r="C9" s="15">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>850</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>1380</v>
+      </c>
+      <c r="O9" s="15">
+        <v>40.050263700000002</v>
+      </c>
+      <c r="P9" s="15">
+        <v>-105.3666599</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>5</v>
+      </c>
+      <c r="S9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="T9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U9" s="15" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="73"/>
+      <c r="B10" s="15" t="s">
+        <v>872</v>
+      </c>
+      <c r="C10" s="15">
+        <v>2020</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>874</v>
+      </c>
+      <c r="M10" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>876</v>
+      </c>
+      <c r="O10" s="15">
+        <v>38.512031</v>
+      </c>
+      <c r="P10" s="15">
+        <v>-122.097228</v>
+      </c>
+      <c r="Q10" s="15">
+        <v>3</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>877</v>
+      </c>
+      <c r="S10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" s="15" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="73"/>
+      <c r="B11" s="15" t="s">
+        <v>882</v>
+      </c>
+      <c r="C11" s="15">
+        <v>2012</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="F11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>884</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>885</v>
+      </c>
+      <c r="O11" s="15">
+        <v>38.896382000000003</v>
+      </c>
+      <c r="P11" s="15">
+        <v>-120.041629</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>2</v>
+      </c>
+      <c r="T11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U11" s="15" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="73"/>
+      <c r="B12" s="15" t="s">
+        <v>897</v>
+      </c>
+      <c r="C12" s="15">
+        <v>2019</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="F12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="73"/>
+      <c r="B13" s="15" t="s">
+        <v>925</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2019</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="F13" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>874</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>927</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>928</v>
+      </c>
+      <c r="O13" s="15">
+        <v>37.534036999999998</v>
+      </c>
+      <c r="P13" s="15">
+        <v>-119.389139</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="T13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U13" s="15" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="73"/>
+      <c r="B14" s="15" t="s">
+        <v>983</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2019</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="F14" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>986</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>695</v>
+      </c>
+      <c r="O14" s="15">
+        <v>39.177683000000002</v>
+      </c>
+      <c r="P14" s="15">
+        <v>-105.26552</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>2</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>985</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" s="15" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="73"/>
+      <c r="B15" s="27" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2015</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>482</v>
+      </c>
+      <c r="F15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>1185</v>
+      </c>
+      <c r="K15" s="49"/>
+      <c r="M15" s="15">
+        <v>4</v>
+      </c>
+      <c r="N15" s="50" t="s">
+        <v>1187</v>
+      </c>
+      <c r="O15" s="15">
+        <v>44.910800000000002</v>
+      </c>
+      <c r="P15" s="15">
+        <v>-116.1031</v>
+      </c>
+      <c r="S15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U15" s="15" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="73" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>936</v>
+      </c>
+      <c r="C16" s="29">
+        <v>2021</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>937</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="M16" s="29" t="s">
+        <v>938</v>
+      </c>
+      <c r="N16" s="29" t="s">
+        <v>939</v>
+      </c>
+      <c r="O16" s="29">
+        <v>69.166667000000004</v>
+      </c>
+      <c r="P16" s="29">
+        <v>-150.75</v>
+      </c>
+      <c r="Q16" s="29">
+        <v>2</v>
+      </c>
+      <c r="S16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="29" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="73"/>
+      <c r="B17" s="44" t="s">
+        <v>671</v>
+      </c>
+      <c r="C17" s="29">
+        <v>2011</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="O17" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="P17" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="T17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" s="29" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="73"/>
+      <c r="B18" s="29" t="s">
+        <v>670</v>
+      </c>
+      <c r="C18" s="29">
+        <v>2000</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>672</v>
+      </c>
+      <c r="N18" s="29" t="s">
+        <v>673</v>
+      </c>
+      <c r="O18" s="69">
+        <v>44.257795999999999</v>
+      </c>
+      <c r="P18" s="44">
+        <v>-71.319730000000007</v>
+      </c>
+      <c r="Q18" s="29">
+        <v>1</v>
+      </c>
+      <c r="R18" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S18" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" s="29" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="73"/>
+      <c r="B19" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1992</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>669</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9" t="s">
+        <v>682</v>
+      </c>
+      <c r="V19" s="9"/>
+    </row>
+    <row r="20" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="73"/>
+      <c r="B20" s="29" t="s">
+        <v>683</v>
+      </c>
+      <c r="C20" s="29">
+        <v>2003</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>686</v>
+      </c>
+      <c r="L20" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="N20" s="29" t="s">
+        <v>684</v>
+      </c>
+      <c r="O20" s="14">
+        <v>32.848999999999997</v>
+      </c>
+      <c r="P20" s="34">
+        <v>-108.593</v>
+      </c>
+      <c r="Q20" s="29">
+        <v>5</v>
+      </c>
+      <c r="R20" s="29" t="s">
+        <v>685</v>
+      </c>
+      <c r="T20" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20" s="29" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="73"/>
+      <c r="B21" s="29" t="s">
+        <v>689</v>
+      </c>
+      <c r="C21" s="29">
+        <v>2011</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>694</v>
+      </c>
+      <c r="L21" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="29" t="s">
+        <v>695</v>
+      </c>
+      <c r="O21" s="29">
+        <v>39.177683000000002</v>
+      </c>
+      <c r="P21" s="29">
+        <v>-105.26552</v>
+      </c>
+      <c r="Q21" s="29">
+        <v>5</v>
+      </c>
+      <c r="R21" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="T21" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="29" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="73"/>
+      <c r="B22" s="29" t="s">
+        <v>711</v>
+      </c>
+      <c r="C22" s="29">
+        <v>2015</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="L22" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="N22" s="29" t="s">
+        <v>708</v>
+      </c>
+      <c r="O22" s="29">
+        <v>40.033332999999999</v>
+      </c>
+      <c r="P22" s="29">
+        <v>-105.416667</v>
+      </c>
+      <c r="Q22" s="29">
+        <v>3</v>
+      </c>
+      <c r="R22" s="29" t="s">
+        <v>709</v>
+      </c>
+      <c r="S22" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T22" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U22" s="29" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="73"/>
+      <c r="B23" s="29" t="s">
+        <v>720</v>
+      </c>
+      <c r="C23" s="29">
+        <v>2019</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" s="29" t="s">
+        <v>721</v>
+      </c>
+      <c r="O23" s="29">
+        <v>39.177683000000002</v>
+      </c>
+      <c r="P23" s="29">
+        <v>-105.26552</v>
+      </c>
+      <c r="S23" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U23" s="29" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="73"/>
+      <c r="B24" s="24" t="s">
+        <v>747</v>
+      </c>
+      <c r="C24" s="24">
+        <v>1991</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>669</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>1102</v>
+      </c>
+      <c r="U24" s="24" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="73"/>
+      <c r="B25" s="29" t="s">
+        <v>763</v>
+      </c>
+      <c r="C25" s="29">
+        <v>2019</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="37" t="s">
+        <v>786</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>694</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="N25" s="29" t="s">
+        <v>721</v>
+      </c>
+      <c r="O25" s="29">
+        <v>39.177683000000002</v>
+      </c>
+      <c r="P25" s="29">
+        <v>-105.26552</v>
+      </c>
+      <c r="S25" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T25" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U25" s="29" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="73"/>
+      <c r="B26" s="29" t="s">
+        <v>766</v>
+      </c>
+      <c r="C26" s="29">
+        <v>2015</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>771</v>
+      </c>
+      <c r="K26" s="31" t="s">
+        <v>772</v>
+      </c>
+      <c r="L26" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="29">
+        <v>1</v>
+      </c>
+      <c r="N26" s="31" t="s">
+        <v>768</v>
+      </c>
+      <c r="O26" s="32">
+        <v>40.7159999</v>
+      </c>
+      <c r="P26" s="32">
+        <v>-105.23308400000001</v>
+      </c>
+      <c r="Q26" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="R26" s="33" t="s">
+        <v>769</v>
+      </c>
+      <c r="S26" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26" s="29" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="73"/>
+      <c r="B27" s="24" t="s">
+        <v>793</v>
+      </c>
+      <c r="C27" s="24">
+        <v>1996</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>669</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>1102</v>
+      </c>
+      <c r="U27" s="24" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="73"/>
+      <c r="B28" s="29" t="s">
+        <v>802</v>
+      </c>
+      <c r="C28" s="29">
+        <v>2015</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="N28" s="31" t="s">
+        <v>803</v>
+      </c>
+      <c r="O28" s="32">
+        <v>35.841000000000001</v>
+      </c>
+      <c r="P28" s="32">
+        <v>-106.5013</v>
+      </c>
+      <c r="Q28" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="R28" s="29" t="s">
+        <v>804</v>
+      </c>
+      <c r="T28" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" s="29" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="73"/>
+      <c r="B29" s="29" t="s">
+        <v>836</v>
+      </c>
+      <c r="C29" s="29">
+        <v>2018</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="M29" s="29">
+        <v>3</v>
+      </c>
+      <c r="N29" s="29" t="s">
+        <v>837</v>
+      </c>
+      <c r="O29" s="29">
+        <v>61.4</v>
+      </c>
+      <c r="P29" s="29">
+        <v>121.433333</v>
+      </c>
+      <c r="Q29" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="R29" s="29" t="s">
+        <v>743</v>
+      </c>
+      <c r="S29" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U29" s="29" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="73"/>
+      <c r="B30" s="29" t="s">
+        <v>910</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>911</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="M30" s="29" t="s">
+        <v>913</v>
+      </c>
+      <c r="N30" s="29" t="s">
+        <v>695</v>
+      </c>
+      <c r="O30" s="29">
+        <v>39.028229000000003</v>
+      </c>
+      <c r="P30" s="29">
+        <v>-105.17336299999999</v>
+      </c>
+      <c r="Q30" s="29">
+        <v>2</v>
+      </c>
+      <c r="R30" s="29" t="s">
+        <v>914</v>
+      </c>
+      <c r="T30" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U30" s="29" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="73"/>
+      <c r="B31" s="29" t="s">
+        <v>929</v>
+      </c>
+      <c r="C31" s="29">
+        <v>1998</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="J31" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" s="29" t="s">
+        <v>933</v>
+      </c>
+      <c r="M31" s="29" t="s">
+        <v>931</v>
+      </c>
+      <c r="N31" s="29" t="s">
+        <v>932</v>
+      </c>
+      <c r="O31" s="29">
+        <v>44.512999999999998</v>
+      </c>
+      <c r="P31" s="29">
+        <v>-109.98</v>
+      </c>
+      <c r="Q31" s="29">
+        <v>4</v>
+      </c>
+      <c r="R31" s="29" t="s">
+        <v>934</v>
+      </c>
+      <c r="S31" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T31" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U31" s="29" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="73"/>
+      <c r="B32" s="29" t="s">
+        <v>949</v>
+      </c>
+      <c r="C32" s="29">
+        <v>2015</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G32" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="M32" s="29" t="s">
+        <v>931</v>
+      </c>
+      <c r="N32" s="29" t="s">
+        <v>950</v>
+      </c>
+      <c r="O32" s="29">
+        <v>44.578524999999999</v>
+      </c>
+      <c r="P32" s="29">
+        <v>-115.66604</v>
+      </c>
+      <c r="Q32" s="29">
+        <v>4</v>
+      </c>
+      <c r="T32" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U32" s="29" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="73"/>
+      <c r="B33" s="29" t="s">
+        <v>958</v>
+      </c>
+      <c r="C33" s="29">
+        <v>2012</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="M33" s="71"/>
+      <c r="N33" s="29" t="s">
+        <v>950</v>
+      </c>
+      <c r="O33" s="29">
+        <v>44.578524999999999</v>
+      </c>
+      <c r="P33" s="29">
+        <v>-115.66604</v>
+      </c>
+      <c r="U33" s="29" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="73"/>
+      <c r="B34" s="29" t="s">
+        <v>987</v>
+      </c>
+      <c r="C34" s="29">
+        <v>2017</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I34" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="M34" s="29" t="s">
+        <v>988</v>
+      </c>
+      <c r="N34" s="29" t="s">
+        <v>989</v>
+      </c>
+      <c r="O34" s="72">
+        <v>38.317307999999997</v>
+      </c>
+      <c r="P34" s="72">
+        <v>-78.634135000000001</v>
+      </c>
+      <c r="Q34" s="29">
+        <v>1</v>
+      </c>
+      <c r="R34" s="29" t="s">
+        <v>990</v>
+      </c>
+      <c r="S34" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U34" s="29" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="73"/>
+      <c r="B35" s="29" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C35" s="29">
+        <v>2021</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="O35" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="P35" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="U35" s="29" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="73"/>
+      <c r="B36" s="29" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C36" s="29">
+        <v>2020</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I36" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="J36" s="29" t="s">
+        <v>1005</v>
+      </c>
+      <c r="M36" s="29" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N36" s="29" t="s">
+        <v>1381</v>
+      </c>
+      <c r="O36" s="29">
+        <v>35</v>
+      </c>
+      <c r="P36" s="29">
+        <v>-83</v>
+      </c>
+      <c r="Q36" s="29">
+        <v>2</v>
+      </c>
+      <c r="R36" s="29" t="s">
+        <v>990</v>
+      </c>
+      <c r="S36" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T36" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U36" s="29" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="73"/>
+      <c r="B37" s="29" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C37" s="29">
+        <v>2007</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="M37" s="29" t="s">
+        <v>1074</v>
+      </c>
+      <c r="N37" s="29" t="s">
+        <v>1075</v>
+      </c>
+      <c r="O37" s="29">
+        <v>44.355572000000002</v>
+      </c>
+      <c r="P37" s="29">
+        <v>-68.288216000000006</v>
+      </c>
+      <c r="Q37" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="S37" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U37" s="29" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="73"/>
+      <c r="B38" s="24" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C38" s="24">
+        <v>2007</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>401</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>402</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>669</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>1102</v>
+      </c>
+      <c r="U38" s="24" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="73"/>
+      <c r="B39" s="29" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C39" s="29">
+        <v>2021</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G39" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="J39" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="29" t="s">
+        <v>1095</v>
+      </c>
+      <c r="L39" s="29" t="s">
+        <v>1093</v>
+      </c>
+      <c r="M39" s="29" t="s">
+        <v>1094</v>
+      </c>
+      <c r="N39" s="29" t="s">
+        <v>1097</v>
+      </c>
+      <c r="O39" s="29">
+        <v>40.262369999999997</v>
+      </c>
+      <c r="P39" s="29">
+        <v>-105.59080400000001</v>
+      </c>
+      <c r="Q39" s="43">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="U39" s="29" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="73"/>
+      <c r="B40" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C40" s="29">
+        <v>2023</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G40" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="J40" s="29" t="s">
+        <v>1169</v>
+      </c>
+      <c r="L40" s="47" t="s">
+        <v>1167</v>
+      </c>
+      <c r="M40" s="29" t="s">
+        <v>988</v>
+      </c>
+      <c r="N40" s="29" t="s">
+        <v>1168</v>
+      </c>
+      <c r="O40" s="29">
+        <v>38.916015999999999</v>
+      </c>
+      <c r="P40" s="29">
+        <v>-120.281718</v>
+      </c>
+      <c r="Q40" s="29">
+        <v>2</v>
+      </c>
+      <c r="R40" s="29" t="s">
+        <v>1171</v>
+      </c>
+      <c r="S40" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U40" s="29" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="73"/>
+      <c r="B41" s="29" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C41" s="29">
+        <v>2023</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>1107</v>
+      </c>
+      <c r="H41" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="L41" s="29" t="s">
+        <v>1177</v>
+      </c>
+      <c r="M41" s="29" t="s">
+        <v>1178</v>
+      </c>
+      <c r="N41" s="48" t="s">
+        <v>1176</v>
+      </c>
+      <c r="O41" s="29">
+        <v>35.890813000000001</v>
+      </c>
+      <c r="P41" s="29">
+        <v>-106.540854</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>9</v>
+      </c>
+      <c r="S41" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T41" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U41" s="29" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="73"/>
+      <c r="B42" s="64" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C42" s="24">
+        <v>1987</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>652</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>669</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H42" s="65"/>
+      <c r="S42" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="T42" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="U42" s="24" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18:G22" xr:uid="{1FFAF820-4EB2-5446-9CB6-5BBC536C303A}">
+      <formula1>"No fire event, no DOC/NO3, No river, Prescribed Burn, Wrong study design, Maybe"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G17" xr:uid="{2B60CAFB-3646-2347-A8C2-8CA45FC2F465}">
+      <formula1>"No fire event, no DOC/NO3, No river, Prescribed Burn, Maybe"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23:G42" xr:uid="{9EDF3BD7-CE4F-CF43-B979-AEBE4326224A}">
+      <formula1>"Included, No fire event, no DOC/NO3, No river, Prescribed Burn, Wrong study design, Maybe"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4EDC603-3282-6340-BD81-0DFA981250B6}">
   <dimension ref="B2:D8"/>
   <sheetViews>
@@ -26132,7 +28237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6601E5-1AF6-2742-B70F-8EB10EC414EE}">
   <dimension ref="A1:G32"/>
   <sheetViews>

</xml_diff>